<commit_message>
API - Builder class initial checkin
</commit_message>
<xml_diff>
--- a/src/test/resources/data/DESKTOP_WEB/Slang/SlangTestData.xlsx
+++ b/src/test/resources/data/DESKTOP_WEB/Slang/SlangTestData.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="6">
   <si>
     <t>Password</t>
   </si>
@@ -34,6 +34,9 @@
   </si>
   <si>
     <t>SampleTest</t>
+  </si>
+  <si>
+    <t>ValidateSpeechApi</t>
   </si>
 </sst>
 </file>
@@ -363,7 +366,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -371,10 +374,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="B5" sqref="B5:C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -409,8 +412,23 @@
       </c>
     </row>
     <row r="5" spans="1:6">
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="B6" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>3</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Mobile caps - fixes
</commit_message>
<xml_diff>
--- a/src/test/resources/data/DESKTOP_WEB/Slang/SlangTestData.xlsx
+++ b/src/test/resources/data/DESKTOP_WEB/Slang/SlangTestData.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="7">
   <si>
     <t>Password</t>
   </si>
@@ -37,6 +37,9 @@
   </si>
   <si>
     <t>ValidateSpeechApi</t>
+  </si>
+  <si>
+    <t>mobileTest</t>
   </si>
 </sst>
 </file>
@@ -366,7 +369,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -374,10 +377,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5:C6"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -430,6 +433,25 @@
         <v>3</v>
       </c>
     </row>
+    <row r="8" spans="1:6">
+      <c r="A8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="B9" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
Mobile agent checkin - Appium driver modified to Android driver
</commit_message>
<xml_diff>
--- a/src/test/resources/data/DESKTOP_WEB/Slang/SlangTestData.xlsx
+++ b/src/test/resources/data/DESKTOP_WEB/Slang/SlangTestData.xlsx
@@ -39,7 +39,7 @@
     <t>ValidateSpeechApi</t>
   </si>
   <si>
-    <t>mobileTest</t>
+    <t>ValidatePageNavigationOnVoiceInput</t>
   </si>
 </sst>
 </file>
@@ -369,7 +369,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -380,7 +380,7 @@
   <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>

</xml_diff>

<commit_message>
Added hindi utterance tests - airtel mock
</commit_message>
<xml_diff>
--- a/src/test/resources/data/DESKTOP_WEB/Slang/SlangTestData.xlsx
+++ b/src/test/resources/data/DESKTOP_WEB/Slang/SlangTestData.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="8">
   <si>
     <t>Password</t>
   </si>
@@ -39,7 +39,10 @@
     <t>ValidateSpeechApi</t>
   </si>
   <si>
-    <t>ValidatePageNavigationOnVoiceInput</t>
+    <t>airtelAppEnglish</t>
+  </si>
+  <si>
+    <t>airtelAppHindi</t>
   </si>
 </sst>
 </file>
@@ -369,7 +372,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -377,10 +380,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -452,6 +455,25 @@
         <v>3</v>
       </c>
     </row>
+    <row r="12" spans="1:6">
+      <c r="A12" t="s">
+        <v>7</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="B13" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>